<commit_message>
arreglados los bots y comentado el codigo
</commit_message>
<xml_diff>
--- a/static/mediaPOS/POS_HOAS50.xlsx
+++ b/static/mediaPOS/POS_HOAS50.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,134 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
-  <si>
-    <t>6672746</t>
-  </si>
-  <si>
-    <t>MOTTO MIRTA MABEL</t>
-  </si>
-  <si>
-    <t>INSTITUTO NACIONAL DE SERVICIOS SOCIALES PARA JUBILADOS Y PENSIONADOS</t>
-  </si>
-  <si>
-    <t>29872682</t>
-  </si>
-  <si>
-    <t>SOTOYESICA MARIEL</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL UNION PERSONAL DE LA UNION DEL  PERSONAL CIVIL DE LA NACION</t>
-  </si>
-  <si>
-    <t>16366345</t>
-  </si>
-  <si>
-    <t>VALDEZ HUGO HORACIO</t>
-  </si>
-  <si>
-    <t>O.S.P. SAN JUAN</t>
-  </si>
-  <si>
-    <t>13662224</t>
-  </si>
-  <si>
-    <t>RAMIREZ MABEL INES</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DE LOS EMPLEADOS DE COMERCIO Y ACTIVIDADES CIVILES</t>
-  </si>
-  <si>
-    <t>35097805</t>
-  </si>
-  <si>
-    <t>SILVA EMANUEL RICARDO</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DEL PERSONAL DE LA CONSTRUCCION</t>
-  </si>
-  <si>
-    <t>46365130</t>
-  </si>
-  <si>
-    <t>ORTIZ ESTRADA FERNANDO</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DEL PERSONAL DE LA SANIDAD ARGENTINA</t>
-  </si>
-  <si>
-    <t>23938885</t>
-  </si>
-  <si>
-    <t>SCHIAPPA PIETRA LUIS ANTONIO</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL PARA LA ACTIVIDAD DOCENTE</t>
-  </si>
-  <si>
-    <t>45271572</t>
-  </si>
-  <si>
-    <t>MANFREDI ZARBA OCTAVIO</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DEL PERSONAL DE LA CONSTRUCCION ; OBRA SOCIAL DE EJECUTIVOS Y DEL PERSONAL DE DIRECCION DE EMPRESAS ; O.S.P. SANTIAGO DEL ESTERO (IOSEP)</t>
-  </si>
-  <si>
-    <t>18030687</t>
-  </si>
-  <si>
-    <t>SALAS GUILLERMO</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DEL PERSONAL RURAL Y ESTIBADORES DE LA REPUBLICA ARGENTINA</t>
-  </si>
-  <si>
-    <t>17197948</t>
-  </si>
-  <si>
-    <t>BACIGALUPPI CRISTIAN</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DEL PERSONAL DEL AUTOMOVIL  CLUB ARGENTINO ; OBRA SOCIAL DE EJECUTIVOS Y DEL PERSONAL DE DIRECCION DE EMPRESAS</t>
-  </si>
-  <si>
-    <t>48521763</t>
-  </si>
-  <si>
-    <t>FUEGO JOAQUIN</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DE COMISARIOS NAVALES</t>
-  </si>
-  <si>
-    <t>53947871</t>
-  </si>
-  <si>
-    <t>MARTINEZ CIRO EMIR</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DEL PERSONAL ASOCIADO A ASOCIACION MUTUAL SANCOR</t>
-  </si>
-  <si>
-    <t>23913663</t>
-  </si>
-  <si>
-    <t>QUINTANA RICARDO RAUL</t>
-  </si>
-  <si>
-    <t>O.S.P. CHACO (INSSSEP)</t>
-  </si>
-  <si>
-    <t>46017441</t>
-  </si>
-  <si>
-    <t>EPELDE CANDELA MACARENA</t>
-  </si>
-  <si>
-    <t>OBRA SOCIAL DEL PERSONAL DEL PAPEL, CARTON Y QUIMICOS</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,162 +360,7 @@
     <col customWidth="1" max="2" min="2" width="35"/>
     <col customWidth="1" max="3" min="3" width="75"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>